<commit_message>
Get forecasts locally or from rest interface
</commit_message>
<xml_diff>
--- a/io/geotemp/mixed/prices_da_results.xlsx
+++ b/io/geotemp/mixed/prices_da_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22044" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22044" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="prices_da" sheetId="1" r:id="rId1"/>
@@ -619,6 +619,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -983,11 +984,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="121234632"/>
-        <c:axId val="121236200"/>
+        <c:axId val="274087040"/>
+        <c:axId val="274085864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121234632"/>
+        <c:axId val="274087040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,7 +1031,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121236200"/>
+        <c:crossAx val="274085864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1038,7 +1039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121236200"/>
+        <c:axId val="274085864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,6 +1059,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1000" b="0" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>$ per MWh</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1089,7 +1154,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121234632"/>
+        <c:crossAx val="274087040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1103,6 +1168,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1220,6 +1286,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1584,11 +1651,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="121237376"/>
-        <c:axId val="121236592"/>
+        <c:axId val="274085080"/>
+        <c:axId val="274082728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121237376"/>
+        <c:axId val="274085080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1631,7 +1698,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121236592"/>
+        <c:crossAx val="274082728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1639,7 +1706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121236592"/>
+        <c:axId val="274082728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,6 +1726,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1000" b="0" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>$ per MWh</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1690,7 +1821,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121237376"/>
+        <c:crossAx val="274085080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1704,6 +1835,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2208,11 +2340,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="121231104"/>
-        <c:axId val="121231888"/>
+        <c:axId val="274086648"/>
+        <c:axId val="274087824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121231104"/>
+        <c:axId val="274086648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2387,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121231888"/>
+        <c:crossAx val="274087824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2263,7 +2395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121231888"/>
+        <c:axId val="274087824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2283,6 +2415,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1000" b="0" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>$ per MWh</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2314,7 +2510,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121231104"/>
+        <c:crossAx val="274086648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2855,11 +3051,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="121232672"/>
-        <c:axId val="121235416"/>
+        <c:axId val="318287288"/>
+        <c:axId val="318285720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121232672"/>
+        <c:axId val="318287288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2902,7 +3098,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121235416"/>
+        <c:crossAx val="318285720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2910,12 +3106,101 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121235416"/>
+        <c:axId val="318285720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="900" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>$ Per MWh</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2947,7 +3232,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121232672"/>
+        <c:crossAx val="318287288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3467,11 +3752,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="121233848"/>
-        <c:axId val="121229928"/>
+        <c:axId val="318283760"/>
+        <c:axId val="318279840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121233848"/>
+        <c:axId val="318283760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3514,7 +3799,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121229928"/>
+        <c:crossAx val="318279840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3522,12 +3807,68 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121229928"/>
+        <c:axId val="318279840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>$ Per MWh</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3559,7 +3900,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121233848"/>
+        <c:crossAx val="318283760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4090,11 +4431,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="121234240"/>
-        <c:axId val="363082640"/>
+        <c:axId val="318286896"/>
+        <c:axId val="318280624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121234240"/>
+        <c:axId val="318286896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4137,7 +4478,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363082640"/>
+        <c:crossAx val="318280624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4145,7 +4486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="363082640"/>
+        <c:axId val="318280624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4165,6 +4506,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>$ per</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" baseline="0"/>
+                  <a:t> MWh</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4196,7 +4598,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121234240"/>
+        <c:crossAx val="318286896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4704,11 +5106,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="363085384"/>
-        <c:axId val="363088520"/>
+        <c:axId val="318285328"/>
+        <c:axId val="318281800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="363085384"/>
+        <c:axId val="318285328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4751,7 +5153,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363088520"/>
+        <c:crossAx val="318281800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4759,7 +5161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="363088520"/>
+        <c:axId val="318281800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4796,7 +5198,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363085384"/>
+        <c:crossAx val="318285328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9286,8 +9688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M529"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16949,8 +17351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>